<commit_message>
feat: se implemento sistema de comparación multi-periodo completo
</commit_message>
<xml_diff>
--- a/Data/Extracto_prueba.xlsx
+++ b/Data/Extracto_prueba.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\German\Gerssss\IA\Hoteles\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\German\Gerssss\IA\Nueva carpeta\Hoteles\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE5A3626-0FD3-437B-A79F-3DEAD50F0CBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05DB7621-DC67-44B7-8924-92C7EF916EEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3220" yWindow="-10910" windowWidth="19420" windowHeight="10420" xr2:uid="{1224B4C5-8DAE-4381-A3E8-5D9004A18356}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{1224B4C5-8DAE-4381-A3E8-5D9004A18356}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -195,7 +195,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="69">
   <si>
     <r>
       <t xml:space="preserve">Alvear Palace </t>
@@ -274,12 +274,6 @@
       </rPr>
       <t xml:space="preserve"> (Jacuzzi) w/Breakfast served at restaurant</t>
     </r>
-  </si>
-  <si>
-    <t>(1May25 - 30Sep25)</t>
-  </si>
-  <si>
-    <t>(1May26 - 30Sep26)</t>
   </si>
   <si>
     <r>
@@ -2035,6 +2029,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="1" fontId="8" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2043,9 +2040,6 @@
     </xf>
     <xf numFmtId="1" fontId="8" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2517,17 +2511,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F94E3EAF-DC7A-49A7-8B54-64A4EE873B20}">
   <dimension ref="A1:J91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C88" sqref="C88"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="133.5703125" customWidth="1"/>
-    <col min="2" max="2" width="58.140625" customWidth="1"/>
+    <col min="1" max="1" width="133.54296875" customWidth="1"/>
+    <col min="2" max="2" width="58.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="21.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="21.5" x14ac:dyDescent="0.45">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -2540,7 +2534,7 @@
       <c r="I1" s="75"/>
       <c r="J1" s="75"/>
     </row>
-    <row r="2" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="19" x14ac:dyDescent="0.4">
       <c r="A2" s="12" t="s">
         <v>1</v>
       </c>
@@ -2555,7 +2549,7 @@
       <c r="I2" s="75"/>
       <c r="J2" s="75"/>
     </row>
-    <row r="3" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="19" x14ac:dyDescent="0.4">
       <c r="A3" s="17" t="s">
         <v>3</v>
       </c>
@@ -2568,7 +2562,7 @@
       <c r="I3" s="75"/>
       <c r="J3" s="75"/>
     </row>
-    <row r="4" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="19" x14ac:dyDescent="0.4">
       <c r="A4" s="22"/>
       <c r="B4" s="23" t="s">
         <v>4</v>
@@ -2581,7 +2575,7 @@
       <c r="I4" s="75"/>
       <c r="J4" s="75"/>
     </row>
-    <row r="5" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="19" x14ac:dyDescent="0.4">
       <c r="A5" s="24" t="s">
         <v>5</v>
       </c>
@@ -2596,7 +2590,7 @@
       <c r="I5" s="75"/>
       <c r="J5" s="75"/>
     </row>
-    <row r="6" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="19" x14ac:dyDescent="0.4">
       <c r="A6" s="24" t="s">
         <v>7</v>
       </c>
@@ -2611,13 +2605,11 @@
       <c r="I6" s="75"/>
       <c r="J6" s="75"/>
     </row>
-    <row r="7" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="19" x14ac:dyDescent="0.4">
       <c r="A7" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="25" t="s">
-        <v>10</v>
-      </c>
+      <c r="B7" s="25"/>
       <c r="C7" s="19">
         <v>387.5</v>
       </c>
@@ -2632,13 +2624,11 @@
       <c r="I7" s="77"/>
       <c r="J7" s="75"/>
     </row>
-    <row r="8" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="19" x14ac:dyDescent="0.4">
       <c r="A8" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="25" t="s">
-        <v>11</v>
-      </c>
+      <c r="B8" s="25"/>
       <c r="C8" s="19">
         <v>481.25</v>
       </c>
@@ -2653,9 +2643,9 @@
       <c r="I8" s="77"/>
       <c r="J8" s="75"/>
     </row>
-    <row r="9" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="19" x14ac:dyDescent="0.4">
       <c r="A9" s="26" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B9" s="25"/>
       <c r="C9" s="19">
@@ -2672,9 +2662,9 @@
       <c r="I9" s="77"/>
       <c r="J9" s="75"/>
     </row>
-    <row r="10" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="19" x14ac:dyDescent="0.4">
       <c r="A10" s="26" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B10" s="28"/>
       <c r="C10" s="19">
@@ -2691,9 +2681,9 @@
       <c r="I10" s="77"/>
       <c r="J10" s="75"/>
     </row>
-    <row r="11" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="19" x14ac:dyDescent="0.4">
       <c r="A11" s="26" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B11" s="23"/>
       <c r="C11" s="19">
@@ -2710,9 +2700,9 @@
       <c r="I11" s="77"/>
       <c r="J11" s="75"/>
     </row>
-    <row r="12" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="19" x14ac:dyDescent="0.4">
       <c r="A12" s="26" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B12" s="28"/>
       <c r="C12" s="19">
@@ -2729,7 +2719,7 @@
       <c r="I12" s="77"/>
       <c r="J12" s="75"/>
     </row>
-    <row r="13" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="19" x14ac:dyDescent="0.4">
       <c r="A13" s="24"/>
       <c r="B13" s="25"/>
       <c r="C13" s="19"/>
@@ -2740,9 +2730,9 @@
       <c r="I13" s="77"/>
       <c r="J13" s="75"/>
     </row>
-    <row r="14" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="19" x14ac:dyDescent="0.4">
       <c r="A14" s="24" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B14" s="25"/>
       <c r="C14" s="19"/>
@@ -2753,9 +2743,9 @@
       <c r="I14" s="77"/>
       <c r="J14" s="75"/>
     </row>
-    <row r="15" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="19" x14ac:dyDescent="0.4">
       <c r="A15" s="26" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B15" s="18"/>
       <c r="C15" s="19">
@@ -2772,9 +2762,9 @@
       <c r="I15" s="77"/>
       <c r="J15" s="75"/>
     </row>
-    <row r="16" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" ht="19" x14ac:dyDescent="0.4">
       <c r="A16" s="29" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B16" s="30"/>
       <c r="C16" s="19">
@@ -2791,7 +2781,7 @@
       <c r="I16" s="77"/>
       <c r="J16" s="75"/>
     </row>
-    <row r="17" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" ht="19" x14ac:dyDescent="0.4">
       <c r="A17" s="24"/>
       <c r="B17" s="25"/>
       <c r="C17" s="19"/>
@@ -2802,9 +2792,9 @@
       <c r="I17" s="77"/>
       <c r="J17" s="75"/>
     </row>
-    <row r="18" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" ht="19" x14ac:dyDescent="0.4">
       <c r="A18" s="24" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B18" s="25"/>
       <c r="C18" s="19"/>
@@ -2815,9 +2805,9 @@
       <c r="I18" s="77"/>
       <c r="J18" s="75"/>
     </row>
-    <row r="19" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" ht="19" x14ac:dyDescent="0.4">
       <c r="A19" s="26" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B19" s="18"/>
       <c r="C19" s="19">
@@ -2834,9 +2824,9 @@
       <c r="I19" s="77"/>
       <c r="J19" s="75"/>
     </row>
-    <row r="20" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" ht="19" x14ac:dyDescent="0.4">
       <c r="A20" s="26" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B20" s="18"/>
       <c r="C20" s="19">
@@ -2853,9 +2843,9 @@
       <c r="I20" s="77"/>
       <c r="J20" s="75"/>
     </row>
-    <row r="21" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" ht="19" x14ac:dyDescent="0.4">
       <c r="A21" s="24" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B21" s="25"/>
       <c r="C21" s="19">
@@ -2872,9 +2862,9 @@
       <c r="I21" s="77"/>
       <c r="J21" s="75"/>
     </row>
-    <row r="22" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" ht="19" x14ac:dyDescent="0.4">
       <c r="A22" s="24" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B22" s="25"/>
       <c r="C22" s="19">
@@ -2891,9 +2881,9 @@
       <c r="I22" s="77"/>
       <c r="J22" s="75"/>
     </row>
-    <row r="23" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" ht="19" x14ac:dyDescent="0.4">
       <c r="A23" s="24" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B23" s="25"/>
       <c r="C23" s="19">
@@ -2910,21 +2900,21 @@
       <c r="I23" s="77"/>
       <c r="J23" s="75"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="G24" s="75"/>
       <c r="H24" s="75"/>
       <c r="I24" s="75"/>
       <c r="J24" s="75"/>
     </row>
-    <row r="25" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="G25" s="75"/>
       <c r="H25" s="75"/>
       <c r="I25" s="75"/>
       <c r="J25" s="75"/>
     </row>
-    <row r="26" spans="1:10" ht="21.75" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" ht="21.5" x14ac:dyDescent="0.45">
       <c r="A26" s="31" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B26" s="32"/>
       <c r="C26" s="33"/>
@@ -2935,7 +2925,7 @@
       <c r="I26" s="75"/>
       <c r="J26" s="75"/>
     </row>
-    <row r="27" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" ht="19" x14ac:dyDescent="0.4">
       <c r="A27" s="1" t="s">
         <v>1</v>
       </c>
@@ -2950,12 +2940,12 @@
       <c r="I27" s="75"/>
       <c r="J27" s="75"/>
     </row>
-    <row r="28" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" ht="19" x14ac:dyDescent="0.4">
       <c r="A28" s="39" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B28" s="40" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C28" s="41"/>
       <c r="D28" s="4"/>
@@ -2965,9 +2955,9 @@
       <c r="I28" s="75"/>
       <c r="J28" s="75"/>
     </row>
-    <row r="29" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" ht="19" x14ac:dyDescent="0.4">
       <c r="A29" s="42" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B29" s="40"/>
       <c r="C29" s="41">
@@ -2984,9 +2974,9 @@
       <c r="I29" s="79"/>
       <c r="J29" s="75"/>
     </row>
-    <row r="30" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" ht="19" x14ac:dyDescent="0.4">
       <c r="A30" s="42" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B30" s="40"/>
       <c r="C30" s="41">
@@ -3003,9 +2993,9 @@
       <c r="I30" s="79"/>
       <c r="J30" s="75"/>
     </row>
-    <row r="31" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" ht="19" x14ac:dyDescent="0.4">
       <c r="A31" s="42" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B31" s="43"/>
       <c r="C31" s="41">
@@ -3022,9 +3012,9 @@
       <c r="I31" s="79"/>
       <c r="J31" s="75"/>
     </row>
-    <row r="32" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" ht="19" x14ac:dyDescent="0.4">
       <c r="A32" s="42" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B32" s="43"/>
       <c r="C32" s="41">
@@ -3041,9 +3031,9 @@
       <c r="I32" s="79"/>
       <c r="J32" s="75"/>
     </row>
-    <row r="33" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" ht="19" x14ac:dyDescent="0.4">
       <c r="A33" s="42" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B33" s="43"/>
       <c r="C33" s="41">
@@ -3060,9 +3050,9 @@
       <c r="I33" s="79"/>
       <c r="J33" s="75"/>
     </row>
-    <row r="34" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" ht="19" x14ac:dyDescent="0.4">
       <c r="A34" s="42" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B34" s="43"/>
       <c r="C34" s="41">
@@ -3079,9 +3069,9 @@
       <c r="I34" s="79"/>
       <c r="J34" s="75"/>
     </row>
-    <row r="35" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" ht="19" x14ac:dyDescent="0.4">
       <c r="A35" s="42" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B35" s="43"/>
       <c r="C35" s="41">
@@ -3098,7 +3088,7 @@
       <c r="I35" s="79"/>
       <c r="J35" s="75"/>
     </row>
-    <row r="36" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" ht="19" x14ac:dyDescent="0.4">
       <c r="A36" s="42"/>
       <c r="B36" s="43"/>
       <c r="C36" s="41"/>
@@ -3109,9 +3099,9 @@
       <c r="I36" s="79"/>
       <c r="J36" s="75"/>
     </row>
-    <row r="37" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" ht="19" x14ac:dyDescent="0.4">
       <c r="A37" s="44" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B37" s="43"/>
       <c r="C37" s="41"/>
@@ -3122,9 +3112,9 @@
       <c r="I37" s="79"/>
       <c r="J37" s="75"/>
     </row>
-    <row r="38" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" ht="19" x14ac:dyDescent="0.4">
       <c r="A38" s="45" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B38" s="43"/>
       <c r="C38" s="41"/>
@@ -3135,7 +3125,7 @@
       <c r="I38" s="79"/>
       <c r="J38" s="75"/>
     </row>
-    <row r="39" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" ht="19" x14ac:dyDescent="0.4">
       <c r="A39" s="46"/>
       <c r="B39" s="43"/>
       <c r="C39" s="41"/>
@@ -3146,9 +3136,9 @@
       <c r="I39" s="79"/>
       <c r="J39" s="75"/>
     </row>
-    <row r="40" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" ht="19" x14ac:dyDescent="0.4">
       <c r="A40" s="47" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B40" s="43"/>
       <c r="C40" s="41"/>
@@ -3159,7 +3149,7 @@
       <c r="I40" s="79"/>
       <c r="J40" s="75"/>
     </row>
-    <row r="41" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" ht="19" x14ac:dyDescent="0.4">
       <c r="A41" s="47"/>
       <c r="B41" s="43"/>
       <c r="C41" s="41"/>
@@ -3170,9 +3160,9 @@
       <c r="I41" s="79"/>
       <c r="J41" s="75"/>
     </row>
-    <row r="42" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" ht="19" x14ac:dyDescent="0.4">
       <c r="A42" s="39" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B42" s="43"/>
       <c r="C42" s="41"/>
@@ -3183,9 +3173,9 @@
       <c r="I42" s="79"/>
       <c r="J42" s="75"/>
     </row>
-    <row r="43" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" ht="19" x14ac:dyDescent="0.4">
       <c r="A43" s="42" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B43" s="40"/>
       <c r="C43" s="41">
@@ -3202,9 +3192,9 @@
       <c r="I43" s="79"/>
       <c r="J43" s="75"/>
     </row>
-    <row r="44" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" ht="19" x14ac:dyDescent="0.4">
       <c r="A44" s="42" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B44" s="43"/>
       <c r="C44" s="41">
@@ -3221,9 +3211,9 @@
       <c r="I44" s="79"/>
       <c r="J44" s="75"/>
     </row>
-    <row r="45" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" ht="19" x14ac:dyDescent="0.4">
       <c r="A45" s="42" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B45" s="43"/>
       <c r="C45" s="41">
@@ -3240,9 +3230,9 @@
       <c r="I45" s="79"/>
       <c r="J45" s="75"/>
     </row>
-    <row r="46" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" ht="19" x14ac:dyDescent="0.4">
       <c r="A46" s="42" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B46" s="43"/>
       <c r="C46" s="41">
@@ -3259,7 +3249,7 @@
       <c r="I46" s="79"/>
       <c r="J46" s="75"/>
     </row>
-    <row r="47" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" ht="19" x14ac:dyDescent="0.4">
       <c r="A47" s="42"/>
       <c r="B47" s="43"/>
       <c r="C47" s="41"/>
@@ -3270,9 +3260,9 @@
       <c r="I47" s="79"/>
       <c r="J47" s="75"/>
     </row>
-    <row r="48" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" ht="19" x14ac:dyDescent="0.4">
       <c r="A48" s="42" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B48" s="43"/>
       <c r="C48" s="41"/>
@@ -3283,9 +3273,9 @@
       <c r="I48" s="79"/>
       <c r="J48" s="75"/>
     </row>
-    <row r="49" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" ht="19" x14ac:dyDescent="0.4">
       <c r="A49" s="42" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B49" s="43"/>
       <c r="C49" s="41"/>
@@ -3296,7 +3286,7 @@
       <c r="I49" s="75"/>
       <c r="J49" s="75"/>
     </row>
-    <row r="50" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" ht="19" x14ac:dyDescent="0.4">
       <c r="A50" s="48"/>
       <c r="B50" s="43"/>
       <c r="C50" s="41"/>
@@ -3307,9 +3297,9 @@
       <c r="I50" s="75"/>
       <c r="J50" s="75"/>
     </row>
-    <row r="51" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" ht="19" x14ac:dyDescent="0.4">
       <c r="A51" s="47" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B51" s="43"/>
       <c r="C51" s="41"/>
@@ -3320,21 +3310,21 @@
       <c r="I51" s="75"/>
       <c r="J51" s="75"/>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
       <c r="G52" s="75"/>
       <c r="H52" s="75"/>
       <c r="I52" s="75"/>
       <c r="J52" s="75"/>
     </row>
-    <row r="53" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="G53" s="75"/>
       <c r="H53" s="75"/>
       <c r="I53" s="75"/>
       <c r="J53" s="75"/>
     </row>
-    <row r="54" spans="1:10" ht="21.75" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:10" ht="21.5" x14ac:dyDescent="0.45">
       <c r="A54" s="31" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B54" s="71"/>
       <c r="C54" s="72"/>
@@ -3345,7 +3335,7 @@
       <c r="I54" s="75"/>
       <c r="J54" s="75"/>
     </row>
-    <row r="55" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:10" ht="19" x14ac:dyDescent="0.4">
       <c r="A55" s="1" t="s">
         <v>1</v>
       </c>
@@ -3360,10 +3350,10 @@
       <c r="I55" s="75"/>
       <c r="J55" s="75"/>
     </row>
-    <row r="56" spans="1:10" ht="36" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" ht="36" x14ac:dyDescent="0.4">
       <c r="A56" s="52"/>
       <c r="B56" s="53" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C56" s="54"/>
       <c r="D56" s="55"/>
@@ -3373,12 +3363,12 @@
       <c r="I56" s="75"/>
       <c r="J56" s="75"/>
     </row>
-    <row r="57" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" ht="19" x14ac:dyDescent="0.4">
       <c r="A57" s="56" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B57" s="57" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C57" s="54"/>
       <c r="D57" s="55"/>
@@ -3388,7 +3378,7 @@
       <c r="I57" s="75"/>
       <c r="J57" s="75"/>
     </row>
-    <row r="58" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" ht="19" x14ac:dyDescent="0.4">
       <c r="A58" s="52"/>
       <c r="B58" s="58"/>
       <c r="C58" s="54"/>
@@ -3399,9 +3389,9 @@
       <c r="I58" s="75"/>
       <c r="J58" s="75"/>
     </row>
-    <row r="59" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:10" ht="19" x14ac:dyDescent="0.4">
       <c r="A59" s="59" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B59" s="60"/>
       <c r="C59" s="61"/>
@@ -3412,12 +3402,12 @@
       <c r="I59" s="75"/>
       <c r="J59" s="75"/>
     </row>
-    <row r="60" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:10" ht="19" x14ac:dyDescent="0.4">
       <c r="A60" s="63" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B60" s="64" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C60" s="54">
         <v>290</v>
@@ -3433,12 +3423,12 @@
       <c r="I60" s="79"/>
       <c r="J60" s="75"/>
     </row>
-    <row r="61" spans="1:10" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" ht="19" x14ac:dyDescent="0.4">
       <c r="A61" s="63" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B61" s="65" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C61" s="54">
         <v>360</v>
@@ -3454,12 +3444,12 @@
       <c r="I61" s="79"/>
       <c r="J61" s="75"/>
     </row>
-    <row r="62" spans="1:10" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" ht="19" x14ac:dyDescent="0.4">
       <c r="A62" s="63" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B62" s="65" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C62" s="54">
         <v>380</v>
@@ -3475,12 +3465,12 @@
       <c r="I62" s="79"/>
       <c r="J62" s="75"/>
     </row>
-    <row r="63" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:10" ht="19" x14ac:dyDescent="0.4">
       <c r="A63" s="63" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B63" s="66" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C63" s="54">
         <v>510</v>
@@ -3496,9 +3486,9 @@
       <c r="I63" s="79"/>
       <c r="J63" s="75"/>
     </row>
-    <row r="64" spans="1:10" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" ht="19" x14ac:dyDescent="0.4">
       <c r="A64" s="67" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B64" s="65"/>
       <c r="C64" s="54">
@@ -3515,9 +3505,9 @@
       <c r="I64" s="79"/>
       <c r="J64" s="75"/>
     </row>
-    <row r="65" spans="1:10" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" ht="19" x14ac:dyDescent="0.4">
       <c r="A65" s="63" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B65" s="65"/>
       <c r="C65" s="54">
@@ -3534,9 +3524,9 @@
       <c r="I65" s="79"/>
       <c r="J65" s="75"/>
     </row>
-    <row r="66" spans="1:10" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" ht="19" x14ac:dyDescent="0.4">
       <c r="A66" s="63" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B66" s="65"/>
       <c r="C66" s="54">
@@ -3553,9 +3543,9 @@
       <c r="I66" s="79"/>
       <c r="J66" s="75"/>
     </row>
-    <row r="67" spans="1:10" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" ht="19" x14ac:dyDescent="0.4">
       <c r="A67" s="63" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B67" s="65"/>
       <c r="C67" s="54">
@@ -3572,9 +3562,9 @@
       <c r="I67" s="79"/>
       <c r="J67" s="75"/>
     </row>
-    <row r="68" spans="1:10" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" ht="19" x14ac:dyDescent="0.4">
       <c r="A68" s="68" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B68" s="65"/>
       <c r="C68" s="54">
@@ -3591,9 +3581,9 @@
       <c r="I68" s="79"/>
       <c r="J68" s="75"/>
     </row>
-    <row r="69" spans="1:10" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" ht="19" x14ac:dyDescent="0.4">
       <c r="A69" s="63" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B69" s="65"/>
       <c r="C69" s="54">
@@ -3610,9 +3600,9 @@
       <c r="I69" s="79"/>
       <c r="J69" s="75"/>
     </row>
-    <row r="70" spans="1:10" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" ht="19" x14ac:dyDescent="0.4">
       <c r="A70" s="63" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B70" s="65"/>
       <c r="C70" s="54">
@@ -3629,9 +3619,9 @@
       <c r="I70" s="79"/>
       <c r="J70" s="75"/>
     </row>
-    <row r="71" spans="1:10" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" ht="19" x14ac:dyDescent="0.4">
       <c r="A71" s="63" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B71" s="65"/>
       <c r="C71" s="54">
@@ -3648,9 +3638,9 @@
       <c r="I71" s="79"/>
       <c r="J71" s="75"/>
     </row>
-    <row r="72" spans="1:10" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" ht="19" x14ac:dyDescent="0.4">
       <c r="A72" s="63" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B72" s="65"/>
       <c r="C72" s="54">
@@ -3667,7 +3657,7 @@
       <c r="I72" s="79"/>
       <c r="J72" s="75"/>
     </row>
-    <row r="73" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" ht="19" x14ac:dyDescent="0.4">
       <c r="A73" s="69"/>
       <c r="B73" s="65"/>
       <c r="C73" s="54"/>
@@ -3678,134 +3668,134 @@
       <c r="I73" s="79"/>
       <c r="J73" s="75"/>
     </row>
-    <row r="74" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:10" ht="19" x14ac:dyDescent="0.4">
       <c r="A74" s="63" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B74" s="64" t="s">
-        <v>50</v>
-      </c>
-      <c r="C74" s="80" t="s">
-        <v>65</v>
-      </c>
-      <c r="D74" s="81"/>
-      <c r="E74" s="82"/>
+        <v>48</v>
+      </c>
+      <c r="C74" s="81" t="s">
+        <v>63</v>
+      </c>
+      <c r="D74" s="82"/>
+      <c r="E74" s="83"/>
       <c r="G74" s="75"/>
       <c r="H74" s="75"/>
       <c r="I74" s="75"/>
       <c r="J74" s="75"/>
     </row>
-    <row r="75" spans="1:10" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" ht="19" x14ac:dyDescent="0.4">
       <c r="A75" s="63" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B75" s="65" t="s">
-        <v>66</v>
-      </c>
-      <c r="C75" s="80"/>
-      <c r="D75" s="81"/>
-      <c r="E75" s="82"/>
+        <v>64</v>
+      </c>
+      <c r="C75" s="81"/>
+      <c r="D75" s="82"/>
+      <c r="E75" s="83"/>
       <c r="G75" s="75"/>
       <c r="H75" s="75"/>
       <c r="I75" s="75"/>
       <c r="J75" s="75"/>
     </row>
-    <row r="76" spans="1:10" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" ht="19" x14ac:dyDescent="0.4">
       <c r="A76" s="63" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B76" s="65"/>
-      <c r="C76" s="80"/>
-      <c r="D76" s="81"/>
-      <c r="E76" s="82"/>
+      <c r="C76" s="81"/>
+      <c r="D76" s="82"/>
+      <c r="E76" s="83"/>
       <c r="G76" s="75"/>
       <c r="H76" s="75"/>
       <c r="I76" s="75"/>
       <c r="J76" s="75"/>
     </row>
-    <row r="77" spans="1:10" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:10" ht="19" x14ac:dyDescent="0.4">
       <c r="A77" s="63" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B77" s="66" t="s">
-        <v>45</v>
-      </c>
-      <c r="C77" s="80"/>
-      <c r="D77" s="81"/>
-      <c r="E77" s="82"/>
+        <v>43</v>
+      </c>
+      <c r="C77" s="81"/>
+      <c r="D77" s="82"/>
+      <c r="E77" s="83"/>
       <c r="G77" s="75"/>
       <c r="H77" s="75"/>
       <c r="I77" s="75"/>
       <c r="J77" s="75"/>
     </row>
-    <row r="78" spans="1:10" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" ht="19" x14ac:dyDescent="0.4">
       <c r="A78" s="67" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B78" s="65"/>
-      <c r="C78" s="80"/>
-      <c r="D78" s="81"/>
-      <c r="E78" s="82"/>
+      <c r="C78" s="81"/>
+      <c r="D78" s="82"/>
+      <c r="E78" s="83"/>
       <c r="G78" s="75"/>
       <c r="H78" s="75"/>
       <c r="I78" s="75"/>
       <c r="J78" s="75"/>
     </row>
-    <row r="79" spans="1:10" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" ht="19" x14ac:dyDescent="0.4">
       <c r="A79" s="63" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B79" s="65"/>
-      <c r="C79" s="80"/>
-      <c r="D79" s="81"/>
-      <c r="E79" s="82"/>
+      <c r="C79" s="81"/>
+      <c r="D79" s="82"/>
+      <c r="E79" s="83"/>
       <c r="G79" s="75"/>
       <c r="H79" s="75"/>
       <c r="I79" s="75"/>
       <c r="J79" s="75"/>
     </row>
-    <row r="80" spans="1:10" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" ht="19" x14ac:dyDescent="0.4">
       <c r="A80" s="63" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B80" s="65"/>
-      <c r="C80" s="80"/>
-      <c r="D80" s="81"/>
-      <c r="E80" s="82"/>
+      <c r="C80" s="81"/>
+      <c r="D80" s="82"/>
+      <c r="E80" s="83"/>
       <c r="G80" s="75"/>
       <c r="H80" s="75"/>
       <c r="I80" s="75"/>
       <c r="J80" s="75"/>
     </row>
-    <row r="81" spans="1:10" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" ht="19" x14ac:dyDescent="0.4">
       <c r="A81" s="63" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B81" s="65"/>
-      <c r="C81" s="80"/>
-      <c r="D81" s="81"/>
-      <c r="E81" s="82"/>
+      <c r="C81" s="81"/>
+      <c r="D81" s="82"/>
+      <c r="E81" s="83"/>
       <c r="G81" s="75"/>
       <c r="H81" s="75"/>
       <c r="I81" s="75"/>
       <c r="J81" s="75"/>
     </row>
-    <row r="82" spans="1:10" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" ht="19" x14ac:dyDescent="0.4">
       <c r="A82" s="68" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B82" s="65"/>
-      <c r="C82" s="80"/>
-      <c r="D82" s="81"/>
-      <c r="E82" s="82"/>
+      <c r="C82" s="81"/>
+      <c r="D82" s="82"/>
+      <c r="E82" s="83"/>
       <c r="G82" s="75"/>
       <c r="H82" s="75"/>
       <c r="I82" s="75"/>
       <c r="J82" s="75"/>
     </row>
-    <row r="83" spans="1:10" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" ht="19" x14ac:dyDescent="0.4">
       <c r="A83" s="63" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B83" s="65"/>
       <c r="C83" s="54">
@@ -3822,9 +3812,9 @@
       <c r="I83" s="79"/>
       <c r="J83" s="75"/>
     </row>
-    <row r="84" spans="1:10" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" ht="19" x14ac:dyDescent="0.4">
       <c r="A84" s="63" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B84" s="65"/>
       <c r="C84" s="54">
@@ -3841,9 +3831,9 @@
       <c r="I84" s="79"/>
       <c r="J84" s="75"/>
     </row>
-    <row r="85" spans="1:10" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" ht="19" x14ac:dyDescent="0.4">
       <c r="A85" s="63" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B85" s="65"/>
       <c r="C85" s="54">
@@ -3860,9 +3850,9 @@
       <c r="I85" s="79"/>
       <c r="J85" s="75"/>
     </row>
-    <row r="86" spans="1:10" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" ht="19" x14ac:dyDescent="0.4">
       <c r="A86" s="63" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B86" s="65"/>
       <c r="C86" s="54">
@@ -3879,21 +3869,21 @@
       <c r="I86" s="79"/>
       <c r="J86" s="75"/>
     </row>
-    <row r="87" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A87" s="83" t="s">
-        <v>68</v>
+    <row r="87" spans="1:10" ht="19" x14ac:dyDescent="0.35">
+      <c r="A87" s="80" t="s">
+        <v>66</v>
       </c>
       <c r="C87" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G87" s="75"/>
       <c r="H87" s="75"/>
       <c r="I87" s="75"/>
       <c r="J87" s="75"/>
     </row>
-    <row r="88" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A88" s="83" t="s">
-        <v>70</v>
+    <row r="88" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+      <c r="A88" s="80" t="s">
+        <v>68</v>
       </c>
       <c r="C88" s="76">
         <v>2500.4499999999998</v>
@@ -3903,19 +3893,19 @@
       <c r="I88" s="75"/>
       <c r="J88" s="75"/>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
       <c r="G89" s="75"/>
       <c r="H89" s="75"/>
       <c r="I89" s="75"/>
       <c r="J89" s="75"/>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
       <c r="G90" s="75"/>
       <c r="H90" s="75"/>
       <c r="I90" s="75"/>
       <c r="J90" s="75"/>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
       <c r="G91" s="75"/>
       <c r="H91" s="75"/>
       <c r="I91" s="75"/>

</xml_diff>

<commit_message>
fix: se corrije la ejecucion de la comparacion de precios. Funciona con multiperiodos.
</commit_message>
<xml_diff>
--- a/Data/Extracto_prueba.xlsx
+++ b/Data/Extracto_prueba.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\German\Gerssss\IA\Nueva carpeta\Hoteles\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\German Lucero\ProyectosChino\Crawl-Compare\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05DB7621-DC67-44B7-8924-92C7EF916EEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1FCD893-B3E7-4648-8912-2C5DE305FD04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{1224B4C5-8DAE-4381-A3E8-5D9004A18356}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1224B4C5-8DAE-4381-A3E8-5D9004A18356}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -195,7 +195,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="70">
   <si>
     <r>
       <t xml:space="preserve">Alvear Palace </t>
@@ -1313,6 +1313,9 @@
   </si>
   <si>
     <t>Habitacion de Prueba2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(1Oct26 - 30Dec26) </t>
   </si>
 </sst>
 </file>
@@ -2512,16 +2515,16 @@
   <dimension ref="A1:J91"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="133.54296875" customWidth="1"/>
-    <col min="2" max="2" width="58.1796875" customWidth="1"/>
+    <col min="1" max="1" width="133.5546875" customWidth="1"/>
+    <col min="2" max="2" width="58.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="21.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -2534,7 +2537,7 @@
       <c r="I1" s="75"/>
       <c r="J1" s="75"/>
     </row>
-    <row r="2" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
         <v>1</v>
       </c>
@@ -2549,7 +2552,7 @@
       <c r="I2" s="75"/>
       <c r="J2" s="75"/>
     </row>
-    <row r="3" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
       <c r="A3" s="17" t="s">
         <v>3</v>
       </c>
@@ -2562,7 +2565,7 @@
       <c r="I3" s="75"/>
       <c r="J3" s="75"/>
     </row>
-    <row r="4" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
       <c r="A4" s="22"/>
       <c r="B4" s="23" t="s">
         <v>4</v>
@@ -2575,7 +2578,7 @@
       <c r="I4" s="75"/>
       <c r="J4" s="75"/>
     </row>
-    <row r="5" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
       <c r="A5" s="24" t="s">
         <v>5</v>
       </c>
@@ -2590,7 +2593,7 @@
       <c r="I5" s="75"/>
       <c r="J5" s="75"/>
     </row>
-    <row r="6" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
       <c r="A6" s="24" t="s">
         <v>7</v>
       </c>
@@ -2605,11 +2608,13 @@
       <c r="I6" s="75"/>
       <c r="J6" s="75"/>
     </row>
-    <row r="7" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
       <c r="A7" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="25"/>
+      <c r="B7" s="25" t="s">
+        <v>69</v>
+      </c>
       <c r="C7" s="19">
         <v>387.5</v>
       </c>
@@ -2624,7 +2629,7 @@
       <c r="I7" s="77"/>
       <c r="J7" s="75"/>
     </row>
-    <row r="8" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
       <c r="A8" s="26" t="s">
         <v>9</v>
       </c>
@@ -2643,7 +2648,7 @@
       <c r="I8" s="77"/>
       <c r="J8" s="75"/>
     </row>
-    <row r="9" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
       <c r="A9" s="26" t="s">
         <v>10</v>
       </c>
@@ -2662,7 +2667,7 @@
       <c r="I9" s="77"/>
       <c r="J9" s="75"/>
     </row>
-    <row r="10" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
       <c r="A10" s="26" t="s">
         <v>11</v>
       </c>
@@ -2681,7 +2686,7 @@
       <c r="I10" s="77"/>
       <c r="J10" s="75"/>
     </row>
-    <row r="11" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
       <c r="A11" s="26" t="s">
         <v>12</v>
       </c>
@@ -2700,7 +2705,7 @@
       <c r="I11" s="77"/>
       <c r="J11" s="75"/>
     </row>
-    <row r="12" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
       <c r="A12" s="26" t="s">
         <v>13</v>
       </c>
@@ -2719,7 +2724,7 @@
       <c r="I12" s="77"/>
       <c r="J12" s="75"/>
     </row>
-    <row r="13" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
       <c r="A13" s="24"/>
       <c r="B13" s="25"/>
       <c r="C13" s="19"/>
@@ -2730,7 +2735,7 @@
       <c r="I13" s="77"/>
       <c r="J13" s="75"/>
     </row>
-    <row r="14" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
       <c r="A14" s="24" t="s">
         <v>14</v>
       </c>
@@ -2743,7 +2748,7 @@
       <c r="I14" s="77"/>
       <c r="J14" s="75"/>
     </row>
-    <row r="15" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
       <c r="A15" s="26" t="s">
         <v>15</v>
       </c>
@@ -2762,7 +2767,7 @@
       <c r="I15" s="77"/>
       <c r="J15" s="75"/>
     </row>
-    <row r="16" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
       <c r="A16" s="29" t="s">
         <v>16</v>
       </c>
@@ -2781,7 +2786,7 @@
       <c r="I16" s="77"/>
       <c r="J16" s="75"/>
     </row>
-    <row r="17" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
       <c r="A17" s="24"/>
       <c r="B17" s="25"/>
       <c r="C17" s="19"/>
@@ -2792,7 +2797,7 @@
       <c r="I17" s="77"/>
       <c r="J17" s="75"/>
     </row>
-    <row r="18" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
       <c r="A18" s="24" t="s">
         <v>17</v>
       </c>
@@ -2805,7 +2810,7 @@
       <c r="I18" s="77"/>
       <c r="J18" s="75"/>
     </row>
-    <row r="19" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
       <c r="A19" s="26" t="s">
         <v>18</v>
       </c>
@@ -2824,7 +2829,7 @@
       <c r="I19" s="77"/>
       <c r="J19" s="75"/>
     </row>
-    <row r="20" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
       <c r="A20" s="26" t="s">
         <v>19</v>
       </c>
@@ -2843,7 +2848,7 @@
       <c r="I20" s="77"/>
       <c r="J20" s="75"/>
     </row>
-    <row r="21" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
       <c r="A21" s="24" t="s">
         <v>20</v>
       </c>
@@ -2862,7 +2867,7 @@
       <c r="I21" s="77"/>
       <c r="J21" s="75"/>
     </row>
-    <row r="22" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
       <c r="A22" s="24" t="s">
         <v>21</v>
       </c>
@@ -2881,7 +2886,7 @@
       <c r="I22" s="77"/>
       <c r="J22" s="75"/>
     </row>
-    <row r="23" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
       <c r="A23" s="24" t="s">
         <v>22</v>
       </c>
@@ -2900,19 +2905,19 @@
       <c r="I23" s="77"/>
       <c r="J23" s="75"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="G24" s="75"/>
       <c r="H24" s="75"/>
       <c r="I24" s="75"/>
       <c r="J24" s="75"/>
     </row>
-    <row r="25" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G25" s="75"/>
       <c r="H25" s="75"/>
       <c r="I25" s="75"/>
       <c r="J25" s="75"/>
     </row>
-    <row r="26" spans="1:10" ht="21.5" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:10" ht="21" x14ac:dyDescent="0.35">
       <c r="A26" s="31" t="s">
         <v>23</v>
       </c>
@@ -2925,7 +2930,7 @@
       <c r="I26" s="75"/>
       <c r="J26" s="75"/>
     </row>
-    <row r="27" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>1</v>
       </c>
@@ -2940,7 +2945,7 @@
       <c r="I27" s="75"/>
       <c r="J27" s="75"/>
     </row>
-    <row r="28" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
       <c r="A28" s="39" t="s">
         <v>24</v>
       </c>
@@ -2955,7 +2960,7 @@
       <c r="I28" s="75"/>
       <c r="J28" s="75"/>
     </row>
-    <row r="29" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
       <c r="A29" s="42" t="s">
         <v>26</v>
       </c>
@@ -2974,7 +2979,7 @@
       <c r="I29" s="79"/>
       <c r="J29" s="75"/>
     </row>
-    <row r="30" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
       <c r="A30" s="42" t="s">
         <v>27</v>
       </c>
@@ -2993,7 +2998,7 @@
       <c r="I30" s="79"/>
       <c r="J30" s="75"/>
     </row>
-    <row r="31" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
       <c r="A31" s="42" t="s">
         <v>28</v>
       </c>
@@ -3012,7 +3017,7 @@
       <c r="I31" s="79"/>
       <c r="J31" s="75"/>
     </row>
-    <row r="32" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
       <c r="A32" s="42" t="s">
         <v>29</v>
       </c>
@@ -3031,7 +3036,7 @@
       <c r="I32" s="79"/>
       <c r="J32" s="75"/>
     </row>
-    <row r="33" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
       <c r="A33" s="42" t="s">
         <v>30</v>
       </c>
@@ -3050,7 +3055,7 @@
       <c r="I33" s="79"/>
       <c r="J33" s="75"/>
     </row>
-    <row r="34" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
       <c r="A34" s="42" t="s">
         <v>31</v>
       </c>
@@ -3069,7 +3074,7 @@
       <c r="I34" s="79"/>
       <c r="J34" s="75"/>
     </row>
-    <row r="35" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
       <c r="A35" s="42" t="s">
         <v>32</v>
       </c>
@@ -3088,7 +3093,7 @@
       <c r="I35" s="79"/>
       <c r="J35" s="75"/>
     </row>
-    <row r="36" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
       <c r="A36" s="42"/>
       <c r="B36" s="43"/>
       <c r="C36" s="41"/>
@@ -3099,7 +3104,7 @@
       <c r="I36" s="79"/>
       <c r="J36" s="75"/>
     </row>
-    <row r="37" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
       <c r="A37" s="44" t="s">
         <v>33</v>
       </c>
@@ -3112,7 +3117,7 @@
       <c r="I37" s="79"/>
       <c r="J37" s="75"/>
     </row>
-    <row r="38" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
       <c r="A38" s="45" t="s">
         <v>34</v>
       </c>
@@ -3125,7 +3130,7 @@
       <c r="I38" s="79"/>
       <c r="J38" s="75"/>
     </row>
-    <row r="39" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
       <c r="A39" s="46"/>
       <c r="B39" s="43"/>
       <c r="C39" s="41"/>
@@ -3136,7 +3141,7 @@
       <c r="I39" s="79"/>
       <c r="J39" s="75"/>
     </row>
-    <row r="40" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
       <c r="A40" s="47" t="s">
         <v>35</v>
       </c>
@@ -3149,7 +3154,7 @@
       <c r="I40" s="79"/>
       <c r="J40" s="75"/>
     </row>
-    <row r="41" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
       <c r="A41" s="47"/>
       <c r="B41" s="43"/>
       <c r="C41" s="41"/>
@@ -3160,7 +3165,7 @@
       <c r="I41" s="79"/>
       <c r="J41" s="75"/>
     </row>
-    <row r="42" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
       <c r="A42" s="39" t="s">
         <v>36</v>
       </c>
@@ -3173,7 +3178,7 @@
       <c r="I42" s="79"/>
       <c r="J42" s="75"/>
     </row>
-    <row r="43" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
       <c r="A43" s="42" t="s">
         <v>37</v>
       </c>
@@ -3192,7 +3197,7 @@
       <c r="I43" s="79"/>
       <c r="J43" s="75"/>
     </row>
-    <row r="44" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
       <c r="A44" s="42" t="s">
         <v>38</v>
       </c>
@@ -3211,7 +3216,7 @@
       <c r="I44" s="79"/>
       <c r="J44" s="75"/>
     </row>
-    <row r="45" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
       <c r="A45" s="42" t="s">
         <v>39</v>
       </c>
@@ -3230,7 +3235,7 @@
       <c r="I45" s="79"/>
       <c r="J45" s="75"/>
     </row>
-    <row r="46" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
       <c r="A46" s="42" t="s">
         <v>40</v>
       </c>
@@ -3249,7 +3254,7 @@
       <c r="I46" s="79"/>
       <c r="J46" s="75"/>
     </row>
-    <row r="47" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
       <c r="A47" s="42"/>
       <c r="B47" s="43"/>
       <c r="C47" s="41"/>
@@ -3260,7 +3265,7 @@
       <c r="I47" s="79"/>
       <c r="J47" s="75"/>
     </row>
-    <row r="48" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
       <c r="A48" s="42" t="s">
         <v>41</v>
       </c>
@@ -3273,7 +3278,7 @@
       <c r="I48" s="79"/>
       <c r="J48" s="75"/>
     </row>
-    <row r="49" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
       <c r="A49" s="42" t="s">
         <v>42</v>
       </c>
@@ -3286,7 +3291,7 @@
       <c r="I49" s="75"/>
       <c r="J49" s="75"/>
     </row>
-    <row r="50" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
       <c r="A50" s="48"/>
       <c r="B50" s="43"/>
       <c r="C50" s="41"/>
@@ -3297,7 +3302,7 @@
       <c r="I50" s="75"/>
       <c r="J50" s="75"/>
     </row>
-    <row r="51" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
       <c r="A51" s="47" t="s">
         <v>35</v>
       </c>
@@ -3310,19 +3315,19 @@
       <c r="I51" s="75"/>
       <c r="J51" s="75"/>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="G52" s="75"/>
       <c r="H52" s="75"/>
       <c r="I52" s="75"/>
       <c r="J52" s="75"/>
     </row>
-    <row r="53" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G53" s="75"/>
       <c r="H53" s="75"/>
       <c r="I53" s="75"/>
       <c r="J53" s="75"/>
     </row>
-    <row r="54" spans="1:10" ht="21.5" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:10" ht="21.6" x14ac:dyDescent="0.4">
       <c r="A54" s="31" t="s">
         <v>65</v>
       </c>
@@ -3335,7 +3340,7 @@
       <c r="I54" s="75"/>
       <c r="J54" s="75"/>
     </row>
-    <row r="55" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>1</v>
       </c>
@@ -3350,7 +3355,7 @@
       <c r="I55" s="75"/>
       <c r="J55" s="75"/>
     </row>
-    <row r="56" spans="1:10" ht="36" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:10" ht="34.799999999999997" x14ac:dyDescent="0.3">
       <c r="A56" s="52"/>
       <c r="B56" s="53" t="s">
         <v>43</v>
@@ -3363,7 +3368,7 @@
       <c r="I56" s="75"/>
       <c r="J56" s="75"/>
     </row>
-    <row r="57" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:10" ht="18.600000000000001" x14ac:dyDescent="0.3">
       <c r="A57" s="56" t="s">
         <v>44</v>
       </c>
@@ -3378,7 +3383,7 @@
       <c r="I57" s="75"/>
       <c r="J57" s="75"/>
     </row>
-    <row r="58" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:10" ht="18.600000000000001" x14ac:dyDescent="0.3">
       <c r="A58" s="52"/>
       <c r="B58" s="58"/>
       <c r="C58" s="54"/>
@@ -3389,7 +3394,7 @@
       <c r="I58" s="75"/>
       <c r="J58" s="75"/>
     </row>
-    <row r="59" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
       <c r="A59" s="59" t="s">
         <v>46</v>
       </c>
@@ -3402,7 +3407,7 @@
       <c r="I59" s="75"/>
       <c r="J59" s="75"/>
     </row>
-    <row r="60" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
       <c r="A60" s="63" t="s">
         <v>47</v>
       </c>
@@ -3423,7 +3428,7 @@
       <c r="I60" s="79"/>
       <c r="J60" s="75"/>
     </row>
-    <row r="61" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:10" ht="19.2" x14ac:dyDescent="0.3">
       <c r="A61" s="63" t="s">
         <v>49</v>
       </c>
@@ -3444,7 +3449,7 @@
       <c r="I61" s="79"/>
       <c r="J61" s="75"/>
     </row>
-    <row r="62" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:10" ht="19.2" x14ac:dyDescent="0.3">
       <c r="A62" s="63" t="s">
         <v>51</v>
       </c>
@@ -3465,7 +3470,7 @@
       <c r="I62" s="79"/>
       <c r="J62" s="75"/>
     </row>
-    <row r="63" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
       <c r="A63" s="63" t="s">
         <v>53</v>
       </c>
@@ -3486,7 +3491,7 @@
       <c r="I63" s="79"/>
       <c r="J63" s="75"/>
     </row>
-    <row r="64" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:10" ht="19.2" x14ac:dyDescent="0.3">
       <c r="A64" s="67" t="s">
         <v>54</v>
       </c>
@@ -3505,7 +3510,7 @@
       <c r="I64" s="79"/>
       <c r="J64" s="75"/>
     </row>
-    <row r="65" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:10" ht="19.2" x14ac:dyDescent="0.3">
       <c r="A65" s="63" t="s">
         <v>55</v>
       </c>
@@ -3524,7 +3529,7 @@
       <c r="I65" s="79"/>
       <c r="J65" s="75"/>
     </row>
-    <row r="66" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:10" ht="19.2" x14ac:dyDescent="0.3">
       <c r="A66" s="63" t="s">
         <v>56</v>
       </c>
@@ -3543,7 +3548,7 @@
       <c r="I66" s="79"/>
       <c r="J66" s="75"/>
     </row>
-    <row r="67" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:10" ht="19.2" x14ac:dyDescent="0.3">
       <c r="A67" s="63" t="s">
         <v>57</v>
       </c>
@@ -3562,7 +3567,7 @@
       <c r="I67" s="79"/>
       <c r="J67" s="75"/>
     </row>
-    <row r="68" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:10" ht="19.2" x14ac:dyDescent="0.3">
       <c r="A68" s="68" t="s">
         <v>58</v>
       </c>
@@ -3581,7 +3586,7 @@
       <c r="I68" s="79"/>
       <c r="J68" s="75"/>
     </row>
-    <row r="69" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:10" ht="19.2" x14ac:dyDescent="0.3">
       <c r="A69" s="63" t="s">
         <v>59</v>
       </c>
@@ -3600,7 +3605,7 @@
       <c r="I69" s="79"/>
       <c r="J69" s="75"/>
     </row>
-    <row r="70" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:10" ht="19.2" x14ac:dyDescent="0.3">
       <c r="A70" s="63" t="s">
         <v>60</v>
       </c>
@@ -3619,7 +3624,7 @@
       <c r="I70" s="79"/>
       <c r="J70" s="75"/>
     </row>
-    <row r="71" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:10" ht="19.2" x14ac:dyDescent="0.3">
       <c r="A71" s="63" t="s">
         <v>61</v>
       </c>
@@ -3638,7 +3643,7 @@
       <c r="I71" s="79"/>
       <c r="J71" s="75"/>
     </row>
-    <row r="72" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:10" ht="19.2" x14ac:dyDescent="0.3">
       <c r="A72" s="63" t="s">
         <v>62</v>
       </c>
@@ -3657,7 +3662,7 @@
       <c r="I72" s="79"/>
       <c r="J72" s="75"/>
     </row>
-    <row r="73" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:10" ht="18.600000000000001" x14ac:dyDescent="0.3">
       <c r="A73" s="69"/>
       <c r="B73" s="65"/>
       <c r="C73" s="54"/>
@@ -3668,7 +3673,7 @@
       <c r="I73" s="79"/>
       <c r="J73" s="75"/>
     </row>
-    <row r="74" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
       <c r="A74" s="63" t="s">
         <v>47</v>
       </c>
@@ -3685,7 +3690,7 @@
       <c r="I74" s="75"/>
       <c r="J74" s="75"/>
     </row>
-    <row r="75" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:10" ht="19.2" x14ac:dyDescent="0.3">
       <c r="A75" s="63" t="s">
         <v>49</v>
       </c>
@@ -3700,7 +3705,7 @@
       <c r="I75" s="75"/>
       <c r="J75" s="75"/>
     </row>
-    <row r="76" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:10" ht="19.2" x14ac:dyDescent="0.3">
       <c r="A76" s="63" t="s">
         <v>51</v>
       </c>
@@ -3713,7 +3718,7 @@
       <c r="I76" s="75"/>
       <c r="J76" s="75"/>
     </row>
-    <row r="77" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:10" ht="19.2" x14ac:dyDescent="0.35">
       <c r="A77" s="63" t="s">
         <v>53</v>
       </c>
@@ -3728,7 +3733,7 @@
       <c r="I77" s="75"/>
       <c r="J77" s="75"/>
     </row>
-    <row r="78" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:10" ht="19.2" x14ac:dyDescent="0.3">
       <c r="A78" s="67" t="s">
         <v>54</v>
       </c>
@@ -3741,7 +3746,7 @@
       <c r="I78" s="75"/>
       <c r="J78" s="75"/>
     </row>
-    <row r="79" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:10" ht="19.2" x14ac:dyDescent="0.3">
       <c r="A79" s="63" t="s">
         <v>55</v>
       </c>
@@ -3754,7 +3759,7 @@
       <c r="I79" s="75"/>
       <c r="J79" s="75"/>
     </row>
-    <row r="80" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:10" ht="19.2" x14ac:dyDescent="0.3">
       <c r="A80" s="63" t="s">
         <v>56</v>
       </c>
@@ -3767,7 +3772,7 @@
       <c r="I80" s="75"/>
       <c r="J80" s="75"/>
     </row>
-    <row r="81" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:10" ht="19.2" x14ac:dyDescent="0.3">
       <c r="A81" s="63" t="s">
         <v>57</v>
       </c>
@@ -3780,7 +3785,7 @@
       <c r="I81" s="75"/>
       <c r="J81" s="75"/>
     </row>
-    <row r="82" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:10" ht="19.2" x14ac:dyDescent="0.3">
       <c r="A82" s="68" t="s">
         <v>58</v>
       </c>
@@ -3793,7 +3798,7 @@
       <c r="I82" s="75"/>
       <c r="J82" s="75"/>
     </row>
-    <row r="83" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:10" ht="19.2" x14ac:dyDescent="0.3">
       <c r="A83" s="63" t="s">
         <v>59</v>
       </c>
@@ -3812,7 +3817,7 @@
       <c r="I83" s="79"/>
       <c r="J83" s="75"/>
     </row>
-    <row r="84" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:10" ht="19.2" x14ac:dyDescent="0.3">
       <c r="A84" s="63" t="s">
         <v>60</v>
       </c>
@@ -3831,7 +3836,7 @@
       <c r="I84" s="79"/>
       <c r="J84" s="75"/>
     </row>
-    <row r="85" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="85" spans="1:10" ht="19.2" x14ac:dyDescent="0.3">
       <c r="A85" s="63" t="s">
         <v>61</v>
       </c>
@@ -3850,7 +3855,7 @@
       <c r="I85" s="79"/>
       <c r="J85" s="75"/>
     </row>
-    <row r="86" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:10" ht="19.2" x14ac:dyDescent="0.3">
       <c r="A86" s="63" t="s">
         <v>62</v>
       </c>
@@ -3869,7 +3874,7 @@
       <c r="I86" s="79"/>
       <c r="J86" s="75"/>
     </row>
-    <row r="87" spans="1:10" ht="19" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:10" ht="18.600000000000001" x14ac:dyDescent="0.3">
       <c r="A87" s="80" t="s">
         <v>66</v>
       </c>
@@ -3881,7 +3886,7 @@
       <c r="I87" s="75"/>
       <c r="J87" s="75"/>
     </row>
-    <row r="88" spans="1:10" ht="19" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:10" ht="18.600000000000001" x14ac:dyDescent="0.3">
       <c r="A88" s="80" t="s">
         <v>68</v>
       </c>
@@ -3893,19 +3898,19 @@
       <c r="I88" s="75"/>
       <c r="J88" s="75"/>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
       <c r="G89" s="75"/>
       <c r="H89" s="75"/>
       <c r="I89" s="75"/>
       <c r="J89" s="75"/>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
       <c r="G90" s="75"/>
       <c r="H90" s="75"/>
       <c r="I90" s="75"/>
       <c r="J90" s="75"/>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
       <c r="G91" s="75"/>
       <c r="H91" s="75"/>
       <c r="I91" s="75"/>

</xml_diff>